<commit_message>
Oscillatory system 1 correct
</commit_message>
<xml_diff>
--- a/Benchmark_System/Oscillatory_System1/Oscillatory System1_dist.xlsx
+++ b/Benchmark_System/Oscillatory_System1/Oscillatory System1_dist.xlsx
@@ -127,7 +127,7 @@
     <col min="2" max="2" width="13.7109375" customWidth="true"/>
     <col min="3" max="3" width="13.7109375" customWidth="true"/>
     <col min="4" max="4" width="13.7109375" customWidth="true"/>
-    <col min="5" max="5" width="12.7109375" customWidth="true"/>
+    <col min="5" max="5" width="14.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -152,16 +152,16 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.10620568033962545</v>
+        <v>0.027006397956728607</v>
       </c>
       <c r="C2">
-        <v>0.10621779866324652</v>
+        <v>0.026893981217712914</v>
       </c>
       <c r="D2">
-        <v>0.10642130270907248</v>
+        <v>0.026903019585067682</v>
       </c>
       <c r="E2">
-        <v>0.56420931454595358</v>
+        <v>0.004364121870257579</v>
       </c>
     </row>
     <row r="3">
@@ -169,16 +169,16 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>9.9990306109839402</v>
+        <v>30.019776248350702</v>
       </c>
       <c r="C3">
-        <v>9.9968948408216303</v>
+        <v>30.018817954391618</v>
       </c>
       <c r="D3">
-        <v>9.9497649759556293</v>
+        <v>30.011538791421234</v>
       </c>
       <c r="E3">
-        <v>3.2928533789917944</v>
+        <v>99.956010938252788</v>
       </c>
     </row>
     <row r="4">
@@ -186,16 +186,16 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.22128372808239669</v>
+        <v>0.1074643643580597</v>
       </c>
       <c r="C4">
-        <v>0.22274072394328648</v>
+        <v>0.10529127196098649</v>
       </c>
       <c r="D4">
-        <v>0.22347161565143708</v>
+        <v>0.10551680732681155</v>
       </c>
       <c r="E4">
-        <v>0.61924973866891142</v>
+        <v>0.10940963220711369</v>
       </c>
     </row>
     <row r="5">
@@ -203,16 +203,16 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>2.1218764250593263</v>
+        <v>1.8299370463193918</v>
       </c>
       <c r="C5">
-        <v>2.1153014384473332</v>
+        <v>1.84734396868327</v>
       </c>
       <c r="D5">
-        <v>2.116520929939707</v>
+        <v>1.8453924521164513</v>
       </c>
       <c r="E5">
-        <v>2.0263808642640417</v>
+        <v>0.9965561804803903</v>
       </c>
     </row>
     <row r="6">
@@ -220,7 +220,7 @@
         <v>5</v>
       </c>
       <c r="E6">
-        <v>112.49795854292654</v>
+        <v>0.013734688769642182</v>
       </c>
     </row>
     <row r="7">
@@ -262,16 +262,16 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>99.995689524618456</v>
+        <v>249.95797553755358</v>
       </c>
       <c r="C9">
-        <v>99.995905661313984</v>
+        <v>249.98667448699553</v>
       </c>
       <c r="D9">
-        <v>99.939286661136947</v>
+        <v>249.98836639623838</v>
       </c>
       <c r="E9">
-        <v>32.999675172655479</v>
+        <v>150.27676897481228</v>
       </c>
     </row>
     <row r="10">
@@ -279,7 +279,7 @@
         <v>9</v>
       </c>
       <c r="E10">
-        <v>0.028158430204651579</v>
+        <v>17.676729830555718</v>
       </c>
     </row>
     <row r="11">
@@ -304,16 +304,16 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>24.429786695062941</v>
+        <v>25.941207743364313</v>
       </c>
       <c r="C12">
-        <v>24.458396937667327</v>
+        <v>26.24061612171343</v>
       </c>
       <c r="D12">
-        <v>24.49644978061049</v>
+        <v>26.253627802783942</v>
       </c>
       <c r="E12">
-        <v>30.728406441565483</v>
+        <v>7.619290605319506</v>
       </c>
     </row>
     <row r="13">
@@ -355,16 +355,16 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>0.040128418840626616</v>
+        <v>0.010734176645309927</v>
       </c>
       <c r="C15">
-        <v>0.040281469390118937</v>
+        <v>0.010606216411124881</v>
       </c>
       <c r="D15">
-        <v>0.040501663057528177</v>
+        <v>0.01062345372257986</v>
       </c>
       <c r="E15">
-        <v>0.16666872663920324</v>
+        <v>0.0041618191671662684</v>
       </c>
     </row>
     <row r="16">
@@ -372,16 +372,16 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>0.98763661040096506</v>
+        <v>0.66435766594882084</v>
       </c>
       <c r="C16">
-        <v>0.9891468607517242</v>
+        <v>0.66138126033990485</v>
       </c>
       <c r="D16">
-        <v>0.99110744702372222</v>
+        <v>0.66180835950768879</v>
       </c>
       <c r="E16">
-        <v>1.6855504335506584</v>
+        <v>0.46492856340000921</v>
       </c>
     </row>
   </sheetData>

</xml_diff>